<commit_message>
MAJ Suivi de projet
</commit_message>
<xml_diff>
--- a/Modelisation/Suivi Projet GestionBrb.xlsx
+++ b/Modelisation/Suivi Projet GestionBrb.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DEE6E6-2065-45E5-88DC-4D2BFB44CB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A437D498-092A-4FEC-A696-ADE223DE623A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1418,7 @@
         <v>37</v>
       </c>
       <c r="J10" s="57">
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="K10" s="16"/>
       <c r="L10" s="17">

</xml_diff>